<commit_message>
Add missing terms and url-links
</commit_message>
<xml_diff>
--- a/#Organisatorisches/Module_Begriffe_Wikipedia-Links.xlsx
+++ b/#Organisatorisches/Module_Begriffe_Wikipedia-Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>1. Semester</t>
   </si>
@@ -363,6 +363,30 @@
   </si>
   <si>
     <t>https://de.wikipedia.org/wiki/Start-up-Unternehmen</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Business_Process_Model_and_Notation</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Marketing-Mix</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Gesch%C3%A4ftsprozessmodellierung</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Gesch%C3%A4ftsprozess</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Werbung</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Algorithmus</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Datenstruktur</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Compiler</t>
   </si>
 </sst>
 </file>
@@ -731,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +849,9 @@
       <c r="P3" t="s">
         <v>83</v>
       </c>
+      <c r="R3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -845,6 +872,9 @@
       <c r="P4" t="s">
         <v>84</v>
       </c>
+      <c r="R4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -865,6 +895,9 @@
       <c r="P5" t="s">
         <v>85</v>
       </c>
+      <c r="R5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -904,6 +937,12 @@
       <c r="H7" t="s">
         <v>98</v>
       </c>
+      <c r="L7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" t="s">
+        <v>43</v>
+      </c>
       <c r="R7" t="s">
         <v>101</v>
       </c>
@@ -921,6 +960,12 @@
       <c r="H8" t="s">
         <v>99</v>
       </c>
+      <c r="L8" t="s">
+        <v>115</v>
+      </c>
+      <c r="P8" t="s">
+        <v>117</v>
+      </c>
       <c r="R8" t="s">
         <v>102</v>
       </c>
@@ -938,6 +983,12 @@
       <c r="H9" t="s">
         <v>100</v>
       </c>
+      <c r="L9" t="s">
+        <v>113</v>
+      </c>
+      <c r="P9" t="s">
+        <v>114</v>
+      </c>
       <c r="R9" t="s">
         <v>103</v>
       </c>
@@ -1151,11 +1202,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A1:B1"/>
@@ -1164,6 +1210,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Dokumentation.docx; Fixing some problems in WikipediaItem.java
</commit_message>
<xml_diff>
--- a/#Organisatorisches/Module_Begriffe_Wikipedia-Links.xlsx
+++ b/#Organisatorisches/Module_Begriffe_Wikipedia-Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
     <t>1. Semester</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Wahlpflichtfächergruppe Informatik</t>
   </si>
   <si>
-    <t>Freiwillige Wahlpflichtfächer</t>
-  </si>
-  <si>
     <t>Produktionswirtschaft</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>https://de.wikipedia.org/wiki/Objektorientierte_Programmierung</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Array</t>
-  </si>
-  <si>
     <t>https://de.wikipedia.org/wiki/Hardware</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>https://de.wikipedia.org/wiki/Rechtsf%C3%A4higkeit</t>
   </si>
   <si>
-    <t>https://de.wikipedia.org/wiki/Datenbank#Datenbankmanagementsystem</t>
-  </si>
-  <si>
     <t>https://de.wikipedia.org/wiki/SQL</t>
   </si>
   <si>
@@ -387,6 +378,12 @@
   </si>
   <si>
     <t>https://de.wikipedia.org/wiki/Compiler</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Feld_(Datentyp)</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Datenbank</t>
   </si>
 </sst>
 </file>
@@ -753,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,9 +766,10 @@
     <col min="8" max="8" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="61.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -800,11 +798,8 @@
       <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -824,82 +819,82 @@
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" t="s">
-        <v>107</v>
-      </c>
-      <c r="P3" t="s">
-        <v>83</v>
-      </c>
-      <c r="R3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" t="s">
-        <v>93</v>
-      </c>
-      <c r="L4" t="s">
-        <v>108</v>
-      </c>
-      <c r="P4" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="R5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -918,82 +913,82 @@
         <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" t="s">
+        <v>114</v>
+      </c>
+      <c r="R8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" t="s">
-        <v>116</v>
-      </c>
-      <c r="P7" t="s">
-        <v>43</v>
-      </c>
-      <c r="R7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>99</v>
-      </c>
-      <c r="L8" t="s">
-        <v>115</v>
-      </c>
-      <c r="P8" t="s">
-        <v>117</v>
-      </c>
-      <c r="R8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>64</v>
-      </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P9" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" t="s">
         <v>100</v>
       </c>
-      <c r="L9" t="s">
-        <v>113</v>
-      </c>
-      <c r="P9" t="s">
-        <v>114</v>
-      </c>
-      <c r="R9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1009,85 +1004,85 @@
         <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
         <v>59</v>
       </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11" t="s">
-        <v>110</v>
-      </c>
-      <c r="P11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" t="s">
-        <v>111</v>
-      </c>
-      <c r="P12" t="s">
-        <v>81</v>
-      </c>
-      <c r="R12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
-      </c>
-      <c r="P13" t="s">
-        <v>82</v>
+        <v>109</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="R13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1100,37 +1095,37 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1148,35 +1143,35 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1187,17 +1182,17 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1221,6 +1216,12 @@
     <hyperlink ref="D11" r:id="rId2"/>
     <hyperlink ref="H11" r:id="rId3"/>
     <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="D20" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="P12" r:id="rId9"/>
+    <hyperlink ref="P13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>